<commit_message>
to do list aktualisiert
</commit_message>
<xml_diff>
--- a/To Do Liste Fopra.xlsx
+++ b/To Do Liste Fopra.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e9eac0077bf55757/Dokumente/_Studium/_Vorlesungen/Fopra/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e9eac0077bf55757/Dokumente/_Studium/_Vorlesungen/Fopra/GIT/Fugaintegrum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="11_AD4DB114E441178AC67DF4CB5651CA40693EDF19" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A08394E2-1A31-4F69-9B1F-C5DBE8C7EABC}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="11_AD4DB114E441178AC67DF4CB5651CA40693EDF19" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{ADD8391A-3332-411A-9164-C89DB6D67B4C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Aufgabe</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Offen</t>
   </si>
   <si>
-    <t>Simulation fixen</t>
-  </si>
-  <si>
     <t>Jakob</t>
   </si>
   <si>
@@ -94,6 +91,21 @@
   </si>
   <si>
     <t>To-Do Liste für offene Projekte</t>
+  </si>
+  <si>
+    <t>Explodierende Vögel</t>
+  </si>
+  <si>
+    <t>offen</t>
+  </si>
+  <si>
+    <t>Simulation fixen (Hindernisse eintragen noch verbuggt)</t>
+  </si>
+  <si>
+    <t>Dronekit studieren</t>
+  </si>
+  <si>
+    <t>GPS der Drohne auslesen</t>
   </si>
 </sst>
 </file>
@@ -161,7 +173,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -173,34 +185,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -489,21 +473,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="46.140625" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="46.1328125" customWidth="1"/>
+    <col min="3" max="3" width="25.1328125" customWidth="1"/>
+    <col min="4" max="4" width="29.1328125" customWidth="1"/>
+    <col min="5" max="5" width="30.265625" customWidth="1"/>
+    <col min="6" max="6" width="27.86328125" customWidth="1"/>
+    <col min="7" max="7" width="32.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -532,10 +516,10 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
@@ -550,25 +534,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D5" s="3">
         <v>44266</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3">
         <v>44266</v>
@@ -576,12 +562,12 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="3">
         <v>44266</v>
@@ -589,24 +575,24 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3">
         <v>44266</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B9" s="2" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>9</v>
@@ -618,25 +604,29 @@
         <v>44271</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="3">
         <v>44266</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="3">
+        <v>44274</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>9</v>
@@ -648,122 +638,142 @@
         <v>44273</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3">
+        <v>44273</v>
+      </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="3">
+        <v>44273</v>
+      </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="3">
+        <v>44273</v>
+      </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>

</xml_diff>

<commit_message>
To Do List updated
</commit_message>
<xml_diff>
--- a/To Do Liste Fopra.xlsx
+++ b/To Do Liste Fopra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e9eac0077bf55757/Dokumente/_Studium/_Vorlesungen/Fopra/GIT/Fugaintegrum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_AD4DB114E441178AC67DF4CB5651CA40693EDF19" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{ADD8391A-3332-411A-9164-C89DB6D67B4C}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="11_AD4DB114E441178AC67DF4CB5651CA40693EDF19" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D4727670-7E2B-4A38-8F23-2909D81CEF22}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>Aufgabe</t>
   </si>
@@ -102,10 +102,22 @@
     <t>Simulation fixen (Hindernisse eintragen noch verbuggt)</t>
   </si>
   <si>
-    <t>Dronekit studieren</t>
-  </si>
-  <si>
     <t>GPS der Drohne auslesen</t>
+  </si>
+  <si>
+    <t>Dronekit  studieren</t>
+  </si>
+  <si>
+    <t>neuen Raspberry aufsetzen</t>
+  </si>
+  <si>
+    <t>neuen Raspberry in Drohne einbauen</t>
+  </si>
+  <si>
+    <t>Martin / Emanuel / … (?)</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -474,7 +486,7 @@
   <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -658,7 +670,7 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3">
@@ -671,7 +683,7 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3">
@@ -683,18 +695,34 @@
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B17" s="2"/>

</xml_diff>

<commit_message>
added Dokumentation, changed To do and deleted Simulation file
</commit_message>
<xml_diff>
--- a/To Do Liste Fopra.xlsx
+++ b/To Do Liste Fopra.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e9eac0077bf55757/Dokumente/_Studium/_Vorlesungen/Fopra/GIT/Fugaintegrum/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e9eac0077bf55757/Dokumente/_Studium/_Vorlesungen/Fopra/GITNEU/Fugaintegrum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="11_AD4DB114E441178AC67DF4CB5651CA40693EDF19" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D4727670-7E2B-4A38-8F23-2909D81CEF22}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="11_AD4DB114E441178AC67DF4CB5651CA40693EDF19" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{502CEF7B-5A7E-488F-8C67-97E80AE65B03}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Aufgabe</t>
   </si>
@@ -48,18 +48,12 @@
     <t>Emanuel</t>
   </si>
   <si>
-    <t>In Arbeit</t>
-  </si>
-  <si>
     <t>Rechercieren wie man Drohne stabiler bekommen</t>
   </si>
   <si>
     <t>Martin</t>
   </si>
   <si>
-    <t>Offen</t>
-  </si>
-  <si>
     <t>Jakob</t>
   </si>
   <si>
@@ -118,6 +112,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>wird wohl leider nie gemacht f</t>
   </si>
 </sst>
 </file>
@@ -486,20 +483,20 @@
   <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.1328125" customWidth="1"/>
-    <col min="3" max="3" width="25.1328125" customWidth="1"/>
-    <col min="4" max="4" width="29.1328125" customWidth="1"/>
-    <col min="5" max="5" width="30.265625" customWidth="1"/>
-    <col min="6" max="6" width="27.86328125" customWidth="1"/>
-    <col min="7" max="7" width="32.73046875" customWidth="1"/>
+    <col min="2" max="2" width="46.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,7 +513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -528,45 +525,45 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="D4" s="3">
         <v>44266</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3">
         <v>44266</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3">
         <v>44266</v>
@@ -574,12 +571,12 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3">
         <v>44266</v>
@@ -587,27 +584,27 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3">
         <v>44266</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="3">
         <v>44266</v>
@@ -616,15 +613,15 @@
         <v>44271</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D10" s="3">
         <v>44266</v>
@@ -633,15 +630,15 @@
         <v>44274</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="3">
         <v>44266</v>
@@ -650,27 +647,29 @@
         <v>44273</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="3">
         <v>44273</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="F12" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3">
@@ -678,12 +677,12 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B14" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3">
@@ -691,117 +690,117 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>

</xml_diff>